<commit_message>
Line Sensor 1st Draft Posted
Line sensor 1st draft for consultation and updated BOM
</commit_message>
<xml_diff>
--- a/docs/UKMARSbotBOM.xlsx
+++ b/docs/UKMARSbotBOM.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian.DELL-PC\Documents\GitHub\ukmarsbot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A019E4-D26D-485F-994A-EE22DC1E8D05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8C300A-0181-465A-96A4-DDD66BE94603}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="110">
   <si>
     <t>Main Board</t>
   </si>
@@ -273,6 +273,102 @@
   </si>
   <si>
     <t>Compatible board</t>
+  </si>
+  <si>
+    <t>Emmitters for line and marker sensing</t>
+  </si>
+  <si>
+    <t>Phototransistors for line and marker sensing</t>
+  </si>
+  <si>
+    <t>Visual Light LEDS for indicators</t>
+  </si>
+  <si>
+    <t>Reservoir de-coupling capacitor</t>
+  </si>
+  <si>
+    <t>100uF ectrolytic 25v, 16v will suffice</t>
+  </si>
+  <si>
+    <t>11-3304</t>
+  </si>
+  <si>
+    <t>SFH4550 IR LEDs or any LED the builder chooses</t>
+  </si>
+  <si>
+    <t>2 Terminal device BPW96B to work with SFH4550 LED or any phototransistor the builder chooses</t>
+  </si>
+  <si>
+    <t>Farnell
+or ebay</t>
+  </si>
+  <si>
+    <t>Farnell 
+RS do packs of 25 much cheaper per unit</t>
+  </si>
+  <si>
+    <t>PN2222A</t>
+  </si>
+  <si>
+    <t>Emmitter driver transistor</t>
+  </si>
+  <si>
+    <t>81-0257</t>
+  </si>
+  <si>
+    <t>Rapid
+ebay and others</t>
+  </si>
+  <si>
+    <t>Emitter resistors</t>
+  </si>
+  <si>
+    <t>Base Resistor</t>
+  </si>
+  <si>
+    <t>R4 value 2K Ohm</t>
+  </si>
+  <si>
+    <t>Sensor Collector Resistors</t>
+  </si>
+  <si>
+    <t>R5 to R8 value 2K Ohm
+Builder may wish to test and adjust</t>
+  </si>
+  <si>
+    <t>R1 to R3 value 68 Ohm
+Builder may wish to test and adjust</t>
+  </si>
+  <si>
+    <t>R9,R10 value 330 Ohm
+Builder may wish to test and adjust</t>
+  </si>
+  <si>
+    <t>Base pull down resistor</t>
+  </si>
+  <si>
+    <t>R11 value 10K Ohm</t>
+  </si>
+  <si>
+    <t>10 pin male header 0.1inch pitch</t>
+  </si>
+  <si>
+    <t>Connector</t>
+  </si>
+  <si>
+    <t>ebay pack of multiple value resistors</t>
+  </si>
+  <si>
+    <t>54-5078</t>
+  </si>
+  <si>
+    <t>Line Sensor pcb</t>
+  </si>
+  <si>
+    <t>Board for all components</t>
+  </si>
+  <si>
+    <t>Not sure of cost</t>
   </si>
 </sst>
 </file>
@@ -325,7 +421,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -466,11 +562,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -530,102 +652,110 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,7 +816,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -738,7 +868,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -940,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,50 +1089,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="35" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="22"/>
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="39"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="23">
-        <v>1</v>
-      </c>
-      <c r="B3" s="21" t="s">
+      <c r="A3" s="48">
+        <v>1</v>
+      </c>
+      <c r="B3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="38" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1014,7 +1144,7 @@
       <c r="F3" s="11">
         <v>3</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="38" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="3">
@@ -1023,9 +1153,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="A4" s="50"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1035,28 +1165,28 @@
       <c r="F4" s="10">
         <v>13</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="48">
         <v>2</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="38" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="40" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="11">
         <v>0.16</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="38" t="s">
         <v>17</v>
       </c>
       <c r="H5" s="3">
@@ -1065,36 +1195,36 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="26"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="10">
         <v>0.16</v>
       </c>
-      <c r="G6" s="22"/>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="G6" s="39"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="48">
         <v>2</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="38" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="27">
+      <c r="E7" s="40"/>
+      <c r="F7" s="52">
         <v>5</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="38" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="3">
@@ -1102,22 +1232,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24"/>
-      <c r="B8" s="22"/>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="50"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="22"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
-        <v>1</v>
-      </c>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="48">
+        <v>1</v>
+      </c>
+      <c r="B9" s="38" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1132,7 +1262,7 @@
       <c r="F9" s="11">
         <v>6.6</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="38" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="3">
@@ -1141,8 +1271,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1155,13 +1285,13 @@
       <c r="F10" s="10">
         <v>6.95</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="39"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
-        <v>1</v>
-      </c>
-      <c r="B11" s="21" t="s">
+      <c r="A11" s="48">
+        <v>1</v>
+      </c>
+      <c r="B11" s="38" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1176,7 +1306,7 @@
       <c r="F11" s="11">
         <v>2.46</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="38" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="3">
@@ -1185,8 +1315,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="4" t="s">
         <v>30</v>
       </c>
@@ -1199,11 +1329,11 @@
       <c r="F12" s="11">
         <v>5.46</v>
       </c>
-      <c r="G12" s="30"/>
+      <c r="G12" s="51"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="51"/>
       <c r="C13" s="20" t="s">
         <v>31</v>
       </c>
@@ -1216,11 +1346,11 @@
       <c r="F13" s="11">
         <v>5.46</v>
       </c>
-      <c r="G13" s="30"/>
+      <c r="G13" s="51"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="22"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="39"/>
       <c r="C14" s="2" t="s">
         <v>75</v>
       </c>
@@ -1229,28 +1359,28 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="22"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>1</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="32" t="s">
         <v>21</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="48">
+      <c r="F15" s="33">
         <v>5</v>
       </c>
-      <c r="G15" s="47" t="s">
+      <c r="G15" s="32" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1279,10 +1409,10 @@
       <c r="A17" s="14">
         <v>2</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="38" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1304,8 +1434,8 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="22"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="2" t="s">
         <v>10</v>
       </c>
@@ -1318,10 +1448,10 @@
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:8" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
-        <v>1</v>
-      </c>
-      <c r="B19" s="34" t="s">
+      <c r="A19" s="48">
+        <v>1</v>
+      </c>
+      <c r="B19" s="45" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -1336,7 +1466,7 @@
       <c r="F19" s="10">
         <v>5.23</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="40" t="s">
         <v>1</v>
       </c>
       <c r="H19" s="3">
@@ -1344,9 +1474,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="29"/>
-      <c r="B20" s="35"/>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="49"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="17" t="s">
         <v>43</v>
       </c>
@@ -1359,11 +1489,11 @@
       <c r="F20" s="10">
         <v>5</v>
       </c>
-      <c r="G20" s="31"/>
-    </row>
-    <row r="21" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="36"/>
+      <c r="G20" s="41"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="50"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="8" t="s">
         <v>44</v>
       </c>
@@ -1376,7 +1506,7 @@
       <c r="F21" s="10">
         <v>10.55</v>
       </c>
-      <c r="G21" s="26"/>
+      <c r="G21" s="42"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
@@ -1536,7 +1666,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13">
         <v>1</v>
       </c>
@@ -1622,109 +1752,348 @@
       <c r="E32" s="5"/>
       <c r="F32" s="10"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="3">
+      <c r="H32" s="54">
         <f>SUM(H3:H30)</f>
         <v>37.31</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="42"/>
-      <c r="B33" s="43" t="s">
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="27"/>
+      <c r="B33" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="44"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="42"/>
-      <c r="B39" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="44"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="29"/>
+    </row>
+    <row r="34" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E34" s="5">
+        <v>1573495</v>
+      </c>
+      <c r="F34" s="10">
+        <v>0.77</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
+        <f t="shared" ref="H34:H38" si="1">A34*MIN(F34)</f>
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="5">
+        <v>1470163</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="1"/>
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="21">
+        <v>1</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.31</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3">
+        <f t="shared" si="1"/>
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="21">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="10">
+        <v>0.12</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3">
+        <f t="shared" si="1"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="21">
+        <v>3</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="10">
+        <v>2.37</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <f>+F39</f>
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="13">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="21">
+        <v>4</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="E41" s="5"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="21">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="21">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F44" s="10">
+        <v>0.67</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3">
+        <f t="shared" ref="H44" si="2">A44*MIN(F44)</f>
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="21">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H45" s="56">
+        <f>SUM(H34:H44)</f>
+        <v>10.31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="21"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="27"/>
+      <c r="B47" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="29"/>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="13"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="2"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="13"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="G11:G14"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
@@ -1740,9 +2109,20 @@
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>